<commit_message>
more rough work for neuroscience club presentation
</commit_message>
<xml_diff>
--- a/doc/regions.xlsx
+++ b/doc/regions.xlsx
@@ -124,9 +124,6 @@
     <t># features</t>
   </si>
   <si>
-    <t>RF diameter</t>
-  </si>
-  <si>
     <t>Rel pixels X features</t>
   </si>
   <si>
@@ -143,6 +140,9 @@
   </si>
   <si>
     <t>order (to distinguish ff and fb connections)</t>
+  </si>
+  <si>
+    <t>RF diameter (pixels)</t>
   </si>
 </sst>
 </file>
@@ -198,8 +198,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -255,7 +275,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="71">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -281,6 +301,16 @@
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -306,6 +336,16 @@
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -638,7 +678,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -657,25 +697,25 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>33</v>
       </c>
-      <c r="G1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" t="s">
         <v>37</v>
-      </c>
-      <c r="K1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -696,29 +736,29 @@
         <v>0.12889999999999999</v>
       </c>
       <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <f>FLOOR(F2/2,1)</f>
+        <v>2</v>
+      </c>
+      <c r="H2">
         <v>364</v>
       </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2">
-        <f>FLOOR(G2/2,1)</f>
-        <v>2</v>
-      </c>
       <c r="I2">
-        <f t="shared" ref="I2:I12" si="1">360*D2/H2</f>
+        <f t="shared" ref="I2:I17" si="1">360*D2/G2</f>
         <v>180</v>
       </c>
       <c r="J2">
-        <f t="shared" ref="J2:J12" si="2">640*D2/H2</f>
+        <f t="shared" ref="J2:J17" si="2">640*D2/G2</f>
         <v>320</v>
       </c>
       <c r="K2">
-        <f>F2*I2*J2</f>
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <f>H2*I2*J2</f>
         <v>20966400</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
       </c>
       <c r="M2" t="s">
         <v>32</v>
@@ -742,16 +782,16 @@
         <v>4.0050000000000002E-2</v>
       </c>
       <c r="F3">
-        <f>ROUND(K3/I3/J3,0)</f>
+        <f t="shared" ref="F3:F21" si="3">C3*F$2</f>
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <f>FLOOR(F3/2,1)</f>
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H17" si="4">ROUND(L3/I3/J3,0)</f>
         <v>1414</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G12" si="3">C3*G$2</f>
-        <v>10</v>
-      </c>
-      <c r="H3">
-        <f>FLOOR(G3/2,1)</f>
-        <v>5</v>
       </c>
       <c r="I3">
         <f t="shared" si="1"/>
@@ -762,14 +802,14 @@
         <v>128</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K12" si="4">K$2*B3/B$2</f>
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <f>L$2*B3/B$2</f>
         <v>13028771.450737007</v>
       </c>
-      <c r="L3">
-        <v>2</v>
-      </c>
       <c r="M3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -790,16 +830,16 @@
         <v>4.0400000000000002E-3</v>
       </c>
       <c r="F4">
-        <f>ROUND(K4/I4/J4,0)</f>
-        <v>16428</v>
-      </c>
-      <c r="G4">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
+      <c r="G4">
+        <f>FLOOR(F4/2,1)</f>
+        <v>12</v>
+      </c>
       <c r="H4">
-        <f>FLOOR(G4/2,1)</f>
-        <v>12</v>
+        <f t="shared" si="4"/>
+        <v>16428</v>
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
@@ -810,11 +850,11 @@
         <v>26.666666666666668</v>
       </c>
       <c r="K4">
-        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <f>L$2*B4/B$2</f>
         <v>6571315.4383242829</v>
-      </c>
-      <c r="L4">
-        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -835,16 +875,16 @@
         <v>3.7000000000000002E-3</v>
       </c>
       <c r="F5">
-        <f>ROUND(K5/I5/J5,0)</f>
-        <v>1045</v>
-      </c>
-      <c r="G5">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G21" si="5">FLOOR(F5/2,1)</f>
+        <v>5</v>
+      </c>
       <c r="H5">
-        <f t="shared" ref="H5:H21" si="5">FLOOR(G5/2,1)</f>
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>1045</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
@@ -855,11 +895,11 @@
         <v>64</v>
       </c>
       <c r="K5">
-        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <f>L$2*B5/B$2</f>
         <v>2407313.5764158266</v>
-      </c>
-      <c r="L5">
-        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -880,16 +920,16 @@
         <v>1.16E-3</v>
       </c>
       <c r="F6">
-        <f>ROUND(K6/I6/J6,0)</f>
-        <v>5118</v>
-      </c>
-      <c r="G6">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="H6">
+      <c r="G6">
         <f t="shared" si="5"/>
         <v>25</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="4"/>
+        <v>5118</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
@@ -900,11 +940,11 @@
         <v>25.6</v>
       </c>
       <c r="K6">
-        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="L6">
+        <f>L$2*B6/B$2</f>
         <v>1886813.3436772693</v>
-      </c>
-      <c r="L6">
-        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -925,16 +965,16 @@
         <v>3.4499999999999998E-4</v>
       </c>
       <c r="F7">
-        <f>ROUND(K7/I7/J7,0)</f>
-        <v>97424</v>
-      </c>
-      <c r="G7">
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="H7">
+      <c r="G7">
         <f t="shared" si="5"/>
         <v>50</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="4"/>
+        <v>97424</v>
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
@@ -945,11 +985,11 @@
         <v>6.4</v>
       </c>
       <c r="K7">
-        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="L7">
+        <f>L$2*B7/B$2</f>
         <v>2244657.2536850274</v>
-      </c>
-      <c r="L7">
-        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -970,16 +1010,16 @@
         <v>9.5000000000000005E-5</v>
       </c>
       <c r="F8">
-        <f>ROUND(K8/I8/J8,0)</f>
-        <v>26827</v>
-      </c>
-      <c r="G8">
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="H8">
+      <c r="G8">
         <f t="shared" si="5"/>
         <v>50</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="4"/>
+        <v>26827</v>
       </c>
       <c r="I8">
         <f t="shared" si="1"/>
@@ -990,11 +1030,11 @@
         <v>6.4</v>
       </c>
       <c r="K8">
-        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="L8">
+        <f>L$2*B8/B$2</f>
         <v>618094.02637703659</v>
-      </c>
-      <c r="L8">
-        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1015,16 +1055,16 @@
         <v>9.2E-5</v>
       </c>
       <c r="F9">
-        <f>ROUND(K9/I9/J9,0)</f>
-        <v>50742</v>
-      </c>
-      <c r="G9">
         <f t="shared" si="3"/>
         <v>250</v>
       </c>
-      <c r="H9">
+      <c r="G9">
         <f t="shared" si="5"/>
         <v>125</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="4"/>
+        <v>50742</v>
       </c>
       <c r="I9">
         <f t="shared" si="1"/>
@@ -1035,11 +1075,11 @@
         <v>5.12</v>
       </c>
       <c r="K9">
-        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="L9">
+        <f>L$2*B9/B$2</f>
         <v>748219.08456167579</v>
-      </c>
-      <c r="L9">
-        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1060,16 +1100,16 @@
         <v>1.3799999999999999E-4</v>
       </c>
       <c r="F10">
-        <f>ROUND(K10/I10/J10,0)</f>
-        <v>76113</v>
-      </c>
-      <c r="G10">
         <f t="shared" si="3"/>
         <v>250</v>
       </c>
-      <c r="H10">
+      <c r="G10">
         <f t="shared" si="5"/>
         <v>125</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="4"/>
+        <v>76113</v>
       </c>
       <c r="I10">
         <f t="shared" si="1"/>
@@ -1080,11 +1120,11 @@
         <v>5.12</v>
       </c>
       <c r="K10">
-        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="L10">
+        <f>L$2*B10/B$2</f>
         <v>1122328.6268425137</v>
-      </c>
-      <c r="L10">
-        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1105,16 +1145,16 @@
         <v>1.0999999999999999E-4</v>
       </c>
       <c r="F11">
-        <f>ROUND(K11/I11/J11,0)</f>
-        <v>60670</v>
-      </c>
-      <c r="G11">
         <f t="shared" si="3"/>
         <v>250</v>
       </c>
-      <c r="H11">
+      <c r="G11">
         <f t="shared" si="5"/>
         <v>125</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="4"/>
+        <v>60670</v>
       </c>
       <c r="I11">
         <f t="shared" si="1"/>
@@ -1125,11 +1165,11 @@
         <v>5.12</v>
       </c>
       <c r="K11">
-        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="L11">
+        <f>L$2*B11/B$2</f>
         <v>894609.77501939493</v>
-      </c>
-      <c r="L11">
-        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -1150,16 +1190,16 @@
         <v>1.3799999999999999E-4</v>
       </c>
       <c r="F12">
-        <f>ROUND(K12/I12/J12,0)</f>
-        <v>76113</v>
-      </c>
-      <c r="G12">
         <f t="shared" si="3"/>
         <v>250</v>
       </c>
-      <c r="H12">
+      <c r="G12">
         <f t="shared" si="5"/>
         <v>125</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="4"/>
+        <v>76113</v>
       </c>
       <c r="I12">
         <f t="shared" si="1"/>
@@ -1170,11 +1210,11 @@
         <v>5.12</v>
       </c>
       <c r="K12">
-        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="L12">
+        <f>L$2*B12/B$2</f>
         <v>1122328.6268425137</v>
-      </c>
-      <c r="L12">
-        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1195,30 +1235,31 @@
         <v>1.25E-4</v>
       </c>
       <c r="F13">
-        <f>ROUND(K13/I13/J13,0)</f>
-        <v>44</v>
-      </c>
-      <c r="G13" s="1">
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="5"/>
+        <v>50</v>
       </c>
       <c r="H13">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>4412</v>
       </c>
       <c r="I13">
-        <f>360*D13/H13</f>
-        <v>72</v>
+        <f t="shared" si="1"/>
+        <v>7.2</v>
       </c>
       <c r="J13">
-        <f>640*D13/H13</f>
-        <v>128</v>
+        <f t="shared" si="2"/>
+        <v>12.8</v>
       </c>
       <c r="K13">
-        <f>K$2*B13/B$2</f>
+        <v>7</v>
+      </c>
+      <c r="L13">
+        <f>L$2*B13/B$2</f>
         <v>406640.80682699772</v>
-      </c>
-      <c r="L13">
-        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -1239,30 +1280,31 @@
         <v>9.2499999999999993E-4</v>
       </c>
       <c r="F14">
-        <f>ROUND(K14/I14/J14,0)</f>
-        <v>327</v>
-      </c>
-      <c r="G14" s="1">
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="5"/>
+        <v>50</v>
       </c>
       <c r="H14">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>32651</v>
       </c>
       <c r="I14">
-        <f>360*D14/H14</f>
-        <v>72</v>
+        <f t="shared" si="1"/>
+        <v>7.2</v>
       </c>
       <c r="J14">
-        <f>640*D14/H14</f>
-        <v>128</v>
+        <f t="shared" si="2"/>
+        <v>12.8</v>
       </c>
       <c r="K14">
-        <f>K$2*B14/B$2</f>
+        <v>6</v>
+      </c>
+      <c r="L14">
+        <f>L$2*B14/B$2</f>
         <v>3009141.970519783</v>
-      </c>
-      <c r="L14">
-        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -1283,30 +1325,31 @@
         <v>5.3333333333333333E-5</v>
       </c>
       <c r="F15">
-        <f>ROUND(K15/I15/J15,0)</f>
-        <v>226</v>
-      </c>
-      <c r="G15" s="1">
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="5"/>
+        <v>75</v>
       </c>
       <c r="H15">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>50830</v>
       </c>
       <c r="I15">
-        <f>360*D15/H15</f>
-        <v>36</v>
+        <f t="shared" si="1"/>
+        <v>2.4</v>
       </c>
       <c r="J15">
-        <f>640*D15/H15</f>
-        <v>64</v>
+        <f t="shared" si="2"/>
+        <v>4.2666666666666666</v>
       </c>
       <c r="K15">
-        <f>K$2*B15/B$2</f>
+        <v>7</v>
+      </c>
+      <c r="L15">
+        <f>L$2*B15/B$2</f>
         <v>520500.23273855716</v>
-      </c>
-      <c r="L15">
-        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1327,30 +1370,31 @@
         <v>2.1499999999999999E-4</v>
       </c>
       <c r="F16">
-        <f>ROUND(K16/I16/J16,0)</f>
-        <v>76</v>
-      </c>
-      <c r="G16" s="1">
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="5"/>
+        <v>50</v>
       </c>
       <c r="H16">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>7589</v>
       </c>
       <c r="I16">
-        <f>360*D16/H16</f>
-        <v>72</v>
+        <f t="shared" si="1"/>
+        <v>7.2</v>
       </c>
       <c r="J16">
-        <f>640*D16/H16</f>
-        <v>128</v>
+        <f t="shared" si="2"/>
+        <v>12.8</v>
       </c>
       <c r="K16">
-        <f>K$2*B16/B$2</f>
+        <v>7</v>
+      </c>
+      <c r="L16">
+        <f>L$2*B16/B$2</f>
         <v>699422.18774243607</v>
-      </c>
-      <c r="L16">
-        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1371,30 +1415,31 @@
         <v>1.1999999999999999E-4</v>
       </c>
       <c r="F17">
-        <f>ROUND(K17/I17/J17,0)</f>
-        <v>42</v>
-      </c>
-      <c r="G17" s="1">
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="5"/>
+        <v>50</v>
       </c>
       <c r="H17">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>4236</v>
       </c>
       <c r="I17">
-        <f>360*D17/H17</f>
-        <v>72</v>
+        <f t="shared" si="1"/>
+        <v>7.2</v>
       </c>
       <c r="J17">
-        <f>640*D17/H17</f>
-        <v>128</v>
+        <f t="shared" si="2"/>
+        <v>12.8</v>
       </c>
       <c r="K17">
-        <f>K$2*B17/B$2</f>
+        <v>6</v>
+      </c>
+      <c r="L17">
+        <f>L$2*B17/B$2</f>
         <v>390375.17455391778</v>
-      </c>
-      <c r="L17">
-        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1407,7 +1452,14 @@
       <c r="C18" t="s">
         <v>30</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="1">
+        <v>100</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="H18">
         <v>1</v>
       </c>
       <c r="I18">
@@ -1416,7 +1468,7 @@
       <c r="J18">
         <v>1</v>
       </c>
-      <c r="L18">
+      <c r="K18">
         <v>8</v>
       </c>
     </row>
@@ -1438,30 +1490,31 @@
         <v>2.7999999999999998E-4</v>
       </c>
       <c r="F19">
-        <f>ROUND(K19/I19/J19,0)</f>
-        <v>99</v>
-      </c>
-      <c r="G19" s="1">
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="5"/>
+        <v>50</v>
       </c>
       <c r="H19">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <f>ROUND(L19/I19/J19,0)</f>
+        <v>9884</v>
       </c>
       <c r="I19">
-        <f>360*D19/H19</f>
-        <v>72</v>
+        <f>360*D19/G19</f>
+        <v>7.2</v>
       </c>
       <c r="J19">
-        <f>640*D19/H19</f>
-        <v>128</v>
+        <f>640*D19/G19</f>
+        <v>12.8</v>
       </c>
       <c r="K19">
-        <f>K$2*B19/B$2</f>
+        <v>7</v>
+      </c>
+      <c r="L19">
+        <f>L$2*B19/B$2</f>
         <v>910875.40729247488</v>
-      </c>
-      <c r="L19">
-        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1478,6 +1531,13 @@
         <v>0.5</v>
       </c>
       <c r="F20">
+        <v>100</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="H20">
         <v>1</v>
       </c>
       <c r="I20">
@@ -1486,7 +1546,7 @@
       <c r="J20">
         <v>1</v>
       </c>
-      <c r="L20">
+      <c r="K20">
         <v>8</v>
       </c>
     </row>
@@ -1508,30 +1568,31 @@
         <v>6.0000000000000006E-4</v>
       </c>
       <c r="F21">
-        <f>ROUND(K21/I21/J21,0)</f>
-        <v>212</v>
-      </c>
-      <c r="G21" s="1">
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="5"/>
+        <v>50</v>
       </c>
       <c r="H21">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <f>ROUND(L21/I21/J21,0)</f>
+        <v>21179</v>
       </c>
       <c r="I21">
-        <f>360*D21/H21</f>
-        <v>72</v>
+        <f>360*D21/G21</f>
+        <v>7.2</v>
       </c>
       <c r="J21">
-        <f>640*D21/H21</f>
-        <v>128</v>
+        <f>640*D21/G21</f>
+        <v>12.8</v>
       </c>
       <c r="K21">
-        <f>K$2*B21/B$2</f>
+        <v>6</v>
+      </c>
+      <c r="L21">
+        <f>L$2*B21/B$2</f>
         <v>1951875.8727695891</v>
-      </c>
-      <c r="L21">
-        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1836,7 +1897,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>